<commit_message>
Plot to Phytochemical Analysis journal.
</commit_message>
<xml_diff>
--- a/Data/Firts_LCMS_Metabolites.xlsx
+++ b/Data/Firts_LCMS_Metabolites.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">RP_NEG_259_013203891066a0_3251741</t>
   </si>
   <si>
-    <t xml:space="preserve">D-(+)-glucose</t>
+    <t xml:space="preserve">Glucose</t>
   </si>
   <si>
     <t xml:space="preserve">Organic oxygen compounds</t>
@@ -312,7 +312,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>